<commit_message>
docs: update calculator_documentation.xlsx for feat: add factorial operation
</commit_message>
<xml_diff>
--- a/docs/calculator_documentation.xlsx
+++ b/docs/calculator_documentation.xlsx
@@ -21,7 +21,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -32,6 +32,11 @@
     <font>
       <b val="1"/>
       <color rgb="00FFFFFF"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <color theme="1"/>
+      <sz val="11"/>
     </font>
   </fonts>
   <fills count="3">
@@ -60,11 +65,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -430,7 +436,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -761,6 +767,212 @@
       <c r="G9" t="inlineStr">
         <is>
           <t>No errors possible</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="inlineStr">
+        <is>
+          <t>Option Number</t>
+        </is>
+      </c>
+      <c r="B10" s="2" t="inlineStr">
+        <is>
+          <t>Option Name</t>
+        </is>
+      </c>
+      <c r="C10" s="2" t="inlineStr">
+        <is>
+          <t>Function</t>
+        </is>
+      </c>
+      <c r="D10" s="2" t="inlineStr">
+        <is>
+          <t>Input Required</t>
+        </is>
+      </c>
+      <c r="E10" s="2" t="inlineStr">
+        <is>
+          <t>Output</t>
+        </is>
+      </c>
+      <c r="F10" s="2" t="inlineStr">
+        <is>
+          <t>Example</t>
+        </is>
+      </c>
+      <c r="G10" s="2" t="inlineStr">
+        <is>
+          <t>Error Handling</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="inlineStr">
+        <is>
+          <t>-------------|-------------|-----------------------------------|----------------------|-----------------------|--------------------------------|--------------</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B12" s="2" t="inlineStr">
+        <is>
+          <t>Addition</t>
+        </is>
+      </c>
+      <c r="C12" s="2" t="inlineStr">
+        <is>
+          <t>Adds two numbers together</t>
+        </is>
+      </c>
+      <c r="D12" s="2" t="inlineStr">
+        <is>
+          <t>Two floating-point...| Sum of the numbers</t>
+        </is>
+      </c>
+      <c r="E12" s="2" t="inlineStr">
+        <is>
+          <t>5.5 + 3.2 = 8.7</t>
+        </is>
+      </c>
+      <c r="F12" s="2" t="inlineStr">
+        <is>
+          <t>Handles invalid input gracefully</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="2" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B13" s="2" t="inlineStr">
+        <is>
+          <t>Subtract</t>
+        </is>
+      </c>
+      <c r="C13" s="2" t="inlineStr">
+        <is>
+          <t>Subt0rctes second number from first| Two floating-point..| Difference of the numb...| 10.0 - 4.5 = 5.5</t>
+        </is>
+      </c>
+      <c r="D13" s="2" t="inlineStr">
+        <is>
+          <t>Handles invalid input gracefully</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="2" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="B14" s="2" t="inlineStr">
+        <is>
+          <t>Multiply</t>
+        </is>
+      </c>
+      <c r="C14" s="2" t="inlineStr">
+        <is>
+          <t>Multiplies two numbers together</t>
+        </is>
+      </c>
+      <c r="D14" s="2" t="inlineStr">
+        <is>
+          <t>Two floating-point..| Product of the numbers| 3.0 * 4.0 = 12.0</t>
+        </is>
+      </c>
+      <c r="E14" s="2" t="inlineStr">
+        <is>
+          <t>Handles invalid input gracefully</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="2" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="B15" s="2" t="inlineStr">
+        <is>
+          <t>Divide</t>
+        </is>
+      </c>
+      <c r="C15" s="2" t="inlineStr">
+        <is>
+          <t>Divides first number by second</t>
+        </is>
+      </c>
+      <c r="D15" s="2" t="inlineStr">
+        <is>
+          <t>Two floating-point..| Quotient of the numb...| 15.0 / 3.0 = 5.0</t>
+        </is>
+      </c>
+      <c r="E15" s="2" t="inlineStr">
+        <is>
+          <t>Raises ValueError for division by zero; handles other errors gracefully</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="2" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="B16" s="2" t="inlineStr">
+        <is>
+          <t>Power</t>
+        </is>
+      </c>
+      <c r="C16" s="2" t="inlineStr">
+        <is>
+          <t>Raises first number to power of se...| Two floating-point..| Result of exponenti...| 2.0 ^ 3.0 = 8.0</t>
+        </is>
+      </c>
+      <c r="D16" s="2" t="inlineStr">
+        <is>
+          <t>Handles invalid input gracefully, including non-numeric inputs and negative results for even roots (raising an error or returning a complex result)</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="2" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="B17" s="2" t="inlineStr">
+        <is>
+          <t>Show History| Displays all previous calculations</t>
+        </is>
+      </c>
+      <c r="C17" s="2" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="D17" s="2" t="inlineStr">
+        <is>
+          <t>List of calculation...</t>
+        </is>
+      </c>
+      <c r="E17" s="2" t="inlineStr">
+        <is>
+          <t>"5.5 + 3.2 = 8.7", ...</t>
+        </is>
+      </c>
+      <c r="F17" s="2" t="inlineStr">
+        <is>
+          <t>Shows the history list, handles empty lists gracefully</t>
         </is>
       </c>
     </row>

</xml_diff>